<commit_message>
Revert "Auxiliary commit to revert individual files from 2a0d9a866ac2654387c803ddf3125034ad9f0868"
This reverts commit 2378d9f595c380943bb7f9ed1e2c86d68ad5ecf6.
</commit_message>
<xml_diff>
--- a/datentool_backend/indicators/tests/testdata/Standorte_und_Kapazitäten.xlsx
+++ b/datentool_backend/indicators/tests/testdata/Standorte_und_Kapazitäten.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\datentool\datentool_backend\indicators\tests\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8C4552-A9DD-4734-AFB0-52B235190AEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4B5FD6-4E33-48CD-B4F9-65CE0FFF4B0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>key</t>
   </si>
@@ -129,9 +129,6 @@
     <t>44b</t>
   </si>
   <si>
-    <t>Place2</t>
-  </si>
-  <si>
     <t>33</t>
   </si>
   <si>
@@ -139,6 +136,24 @@
   </si>
   <si>
     <t>Buchstaben</t>
+  </si>
+  <si>
+    <t>Ort 2</t>
+  </si>
+  <si>
+    <t>Marktplatz</t>
+  </si>
+  <si>
+    <t>Place3</t>
+  </si>
+  <si>
+    <t>Hauptstraße</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Place 4</t>
   </si>
 </sst>
 </file>
@@ -537,7 +552,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,10 +562,10 @@
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -590,13 +605,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
+      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,10 +715,10 @@
         <v>34</v>
       </c>
       <c r="G4">
-        <v>12.3</v>
+        <v>-106.499686</v>
       </c>
       <c r="H4">
-        <v>55.5</v>
+        <v>-78.608621499999998</v>
       </c>
       <c r="I4">
         <v>1234</v>
@@ -726,16 +741,19 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" t="s">
-        <v>36</v>
-      </c>
       <c r="G5">
-        <v>12.4</v>
+        <v>-106.499686</v>
       </c>
       <c r="H5">
-        <v>55.4</v>
+        <v>-78.608621499999998</v>
       </c>
       <c r="I5">
         <v>567</v>
@@ -743,10 +761,71 @@
       <c r="J5" t="s">
         <v>9</v>
       </c>
+      <c r="K5" t="s">
+        <v>8</v>
+      </c>
       <c r="L5">
         <v>0</v>
       </c>
-      <c r="M5">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6">
+        <v>123</v>
+      </c>
+      <c r="E6">
+        <v>12345</v>
+      </c>
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>55</v>
+      </c>
+      <c r="I6">
+        <v>123</v>
+      </c>
+      <c r="J6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7">
+        <v>11</v>
+      </c>
+      <c r="H7">
+        <v>66</v>
+      </c>
+      <c r="I7">
+        <v>123</v>
+      </c>
+      <c r="K7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
         <v>0</v>
       </c>
     </row>
@@ -768,18 +847,30 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Nur Werte aus Liste erlaubt" xr:uid="{00000000-0002-0000-0200-000005000000}">
           <x14:formula1>
             <xm:f>Klassifizierungen!$B$2:$B$9999</xm:f>
           </x14:formula1>
-          <xm:sqref>J3:J999999</xm:sqref>
+          <xm:sqref>J8:J999999</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Nur Werte aus Liste erlaubt" xr:uid="{00000000-0002-0000-0200-000006000000}">
           <x14:formula1>
             <xm:f>Klassifizierungen!$C$2:$C$9999</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K999999</xm:sqref>
+          <xm:sqref>K8:K999999</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Nur Werte aus Liste erlaubt" xr:uid="{B2BA557A-6AAD-4895-A16F-9F8F01E07CCF}">
+          <x14:formula1>
+            <xm:f>[Standorte_und_Kapazitäten_mod.xlsx]Klassifizierungen!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>K3:K7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Nur Werte aus Liste erlaubt" xr:uid="{C7A0E1B8-9259-4DC9-B17F-BE66BB2525A6}">
+          <x14:formula1>
+            <xm:f>[Standorte_und_Kapazitäten_mod.xlsx]Klassifizierungen!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>J3:J7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
PlaceTemplate without empty/hidden rows and columns. PLZ-Column format enforced. Unique-Name enforced
</commit_message>
<xml_diff>
--- a/datentool_backend/indicators/tests/testdata/Standorte_und_Kapazitäten.xlsx
+++ b/datentool_backend/indicators/tests/testdata/Standorte_und_Kapazitäten.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\datentool\datentool_backend\indicators\tests\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\bule_datentool\datentool_backend\indicators\tests\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4B5FD6-4E33-48CD-B4F9-65CE0FFF4B0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EE9ACD-BA16-4D28-BD0A-B73786C3DB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="meta" sheetId="1" r:id="rId1"/>
-    <sheet name="Klassifizierungen" sheetId="2" r:id="rId2"/>
+    <sheet name="meta" sheetId="1" state="hidden" r:id="rId1"/>
+    <sheet name="Klassifizierungen" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="Standorte und Kapazitäten" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -22,23 +22,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
-  <si>
-    <t>key</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>infrastructure</t>
   </si>
   <si>
-    <t>1</t>
+    <t>perspiciatis</t>
   </si>
   <si>
     <t>order</t>
   </si>
   <si>
+    <t>Ziffern</t>
+  </si>
+  <si>
+    <t>Buchstaben</t>
+  </si>
+  <si>
     <t>Eins</t>
   </si>
   <si>
@@ -54,6 +54,9 @@
     <t>Drei</t>
   </si>
   <si>
+    <t>place_id</t>
+  </si>
+  <si>
     <t>Name</t>
   </si>
   <si>
@@ -90,6 +93,9 @@
     <t>Kapazität für Leistung Schulplätze</t>
   </si>
   <si>
+    <t>Hier stehen die daviplan-internen Nummern von bereits hochgeladenen Standorten. Bitte nicht verändern.</t>
+  </si>
+  <si>
     <t>So werden die Einrichtungen auf den Karten beschriftet. Jeder Standort muss einen Namen haben, den kein anderer Standort trägt.</t>
   </si>
   <si>
@@ -108,7 +114,7 @@
     <t>Breitengrad, in WGS84</t>
   </si>
   <si>
-    <t>Nutzerdefinierte Spalte (Zahl)</t>
+    <t>Nutzerdefinierte Spalte (Punkte)</t>
   </si>
   <si>
     <t>Nutzerdefinierte Spalte (Klassifizierte Werte)</t>
@@ -117,43 +123,34 @@
     <t>1 wenn ja, sonst 0</t>
   </si>
   <si>
+    <t>Place1</t>
+  </si>
+  <si>
+    <t>44b</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>Ort 2</t>
+  </si>
+  <si>
+    <t>Marktplatz</t>
+  </si>
+  <si>
+    <t>Place3</t>
+  </si>
+  <si>
+    <t>Hauptstraße</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Place 4</t>
+  </si>
+  <si>
     <t>temporibus</t>
-  </si>
-  <si>
-    <t>place_id</t>
-  </si>
-  <si>
-    <t>Place1</t>
-  </si>
-  <si>
-    <t>44b</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>Ziffern</t>
-  </si>
-  <si>
-    <t>Buchstaben</t>
-  </si>
-  <si>
-    <t>Ort 2</t>
-  </si>
-  <si>
-    <t>Marktplatz</t>
-  </si>
-  <si>
-    <t>Place3</t>
-  </si>
-  <si>
-    <t>Hauptstraße</t>
-  </si>
-  <si>
-    <t>Hamburg</t>
-  </si>
-  <si>
-    <t>Place 4</t>
   </si>
 </sst>
 </file>
@@ -175,12 +172,17 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0C0C0"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -210,14 +212,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -520,26 +526,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -551,25 +549,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -579,8 +575,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -590,8 +586,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -605,114 +601,148 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
     <col min="3" max="13" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="F2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="K2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="M2" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3">
+        <v>-106.499686</v>
+      </c>
+      <c r="H3">
+        <v>-78.608621499999998</v>
+      </c>
+      <c r="I3">
+        <v>1234</v>
+      </c>
+      <c r="J3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>55.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G4">
         <v>-106.499686</v>
@@ -721,156 +751,112 @@
         <v>-78.608621499999998</v>
       </c>
       <c r="I4">
-        <v>1234</v>
+        <v>567</v>
       </c>
       <c r="J4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K4" t="s">
         <v>8</v>
       </c>
       <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>55.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>2</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>38</v>
       </c>
       <c r="C5" t="s">
         <v>39</v>
       </c>
-      <c r="D5" t="s">
-        <v>35</v>
+      <c r="D5">
+        <v>123</v>
+      </c>
+      <c r="E5">
+        <v>12345</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
       </c>
       <c r="G5">
-        <v>-106.499686</v>
+        <v>10</v>
       </c>
       <c r="H5">
-        <v>-78.608621499999998</v>
+        <v>55</v>
       </c>
       <c r="I5">
-        <v>567</v>
+        <v>123</v>
       </c>
       <c r="J5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" t="s">
         <v>41</v>
       </c>
-      <c r="D6">
-        <v>123</v>
-      </c>
-      <c r="E6">
-        <v>12345</v>
-      </c>
-      <c r="F6" t="s">
-        <v>42</v>
-      </c>
       <c r="G6">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H6">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="I6">
         <v>123</v>
       </c>
-      <c r="J6" t="s">
-        <v>7</v>
-      </c>
       <c r="K6" t="s">
         <v>6</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7">
-        <v>11</v>
-      </c>
-      <c r="H7">
-        <v>66</v>
-      </c>
-      <c r="I7">
-        <v>123</v>
-      </c>
-      <c r="K7" t="s">
-        <v>6</v>
-      </c>
-      <c r="L7">
         <v>0</v>
       </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="5">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ungültige Koordinaten" error="Koordinaten müssen in WGS84 angegeben werden und zwischen 0 und 90 liegen" sqref="G3:H999999" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>0</formula1>
       <formula2>90</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Nur 0 oder 1 erlaubt" sqref="L3:L999999" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name nicht eindeutig" error="Name muss eindeutig sein" sqref="B3:B999999" xr:uid="{00000000-0002-0000-0200-000001000000}">
+      <formula1>COUNTIF(B$3:B$99999,B3)&lt;2</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Nur 0 oder 1 erlaubt" sqref="L2:L999999" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Nur Zahlen erlaubt" sqref="I3:I999999" xr:uid="{00000000-0002-0000-0200-000002000000}"/>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Nur Zahlen &gt;= 0 erlaubt" sqref="M3:M999999" xr:uid="{00000000-0002-0000-0200-000003000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Nur Zahlen erlaubt" sqref="I2:I999999" xr:uid="{00000000-0002-0000-0200-000003000000}"/>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Nur Zahlen &gt;= 0 erlaubt" sqref="M3:M999999" xr:uid="{00000000-0002-0000-0200-000004000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Nur Werte aus Liste erlaubt" xr:uid="{00000000-0002-0000-0200-000005000000}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Nur Werte aus Liste erlaubt" xr:uid="{00000000-0002-0000-0200-000006000000}">
           <x14:formula1>
             <xm:f>Klassifizierungen!$B$2:$B$9999</xm:f>
           </x14:formula1>
-          <xm:sqref>J8:J999999</xm:sqref>
+          <xm:sqref>J2:J999999</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Nur Werte aus Liste erlaubt" xr:uid="{00000000-0002-0000-0200-000006000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Nur Werte aus Liste erlaubt" xr:uid="{00000000-0002-0000-0200-000007000000}">
           <x14:formula1>
             <xm:f>Klassifizierungen!$C$2:$C$9999</xm:f>
           </x14:formula1>
-          <xm:sqref>K8:K999999</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Nur Werte aus Liste erlaubt" xr:uid="{B2BA557A-6AAD-4895-A16F-9F8F01E07CCF}">
-          <x14:formula1>
-            <xm:f>[Standorte_und_Kapazitäten_mod.xlsx]Klassifizierungen!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>K3:K7</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Nur Werte aus Liste erlaubt" xr:uid="{C7A0E1B8-9259-4DC9-B17F-BE66BB2525A6}">
-          <x14:formula1>
-            <xm:f>[Standorte_und_Kapazitäten_mod.xlsx]Klassifizierungen!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>J3:J7</xm:sqref>
+          <xm:sqref>K2:K999999</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>